<commit_message>
all sorts of stuff
</commit_message>
<xml_diff>
--- a/notebooks/Data/Solo_A_Star_Wars_Story/centrality.xlsx
+++ b/notebooks/Data/Solo_A_Star_Wars_Story/centrality.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
   <si>
     <t>betweenness_centrality</t>
   </si>
@@ -28,9 +28,15 @@
     <t>eigenvector_centrality</t>
   </si>
   <si>
+    <t>in_degree</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
+    <t>out_degree</t>
+  </si>
+  <si>
     <t>Val</t>
   </si>
   <si>
@@ -67,373 +73,373 @@
     <t>JV-P12</t>
   </si>
   <si>
+    <t>Rebolt</t>
+  </si>
+  <si>
+    <t>Argus Panox</t>
+  </si>
+  <si>
+    <t>R5-PHT</t>
+  </si>
+  <si>
+    <t>Chates</t>
+  </si>
+  <si>
+    <t>Denwade Banevans</t>
+  </si>
+  <si>
+    <t>Needles</t>
+  </si>
+  <si>
+    <t>Waria Junus</t>
+  </si>
+  <si>
+    <t>HT-IN-4</t>
+  </si>
+  <si>
+    <t>Wesger Odry</t>
+  </si>
+  <si>
+    <t>Toht Ra</t>
+  </si>
+  <si>
+    <t>GOUD-4</t>
+  </si>
+  <si>
+    <t>Rio Durant</t>
+  </si>
+  <si>
+    <t>Fugas Fandita</t>
+  </si>
+  <si>
+    <t>Dava Cassamam</t>
+  </si>
+  <si>
+    <t>Crev Bombaasa</t>
+  </si>
+  <si>
+    <t>Ralakili</t>
+  </si>
+  <si>
+    <t>Tobias Beckett</t>
+  </si>
+  <si>
+    <t>Hallon</t>
+  </si>
+  <si>
+    <t>Therm Scissorpunch</t>
+  </si>
+  <si>
+    <t>Ottilie</t>
+  </si>
+  <si>
+    <t>Enfys Nest</t>
+  </si>
+  <si>
+    <t>Damici Stalado</t>
+  </si>
+  <si>
+    <t>1MSE-KUP24</t>
+  </si>
+  <si>
+    <t>Odeffro Msern</t>
+  </si>
+  <si>
+    <t>Han Solo</t>
+  </si>
+  <si>
+    <t>Tak</t>
+  </si>
+  <si>
+    <t>Senna (Gigoran)</t>
+  </si>
+  <si>
+    <t>Proxima</t>
+  </si>
+  <si>
+    <t>Loru Denholt</t>
+  </si>
+  <si>
+    <t>Sinuth</t>
+  </si>
+  <si>
+    <t>Gelan Yees</t>
+  </si>
+  <si>
+    <t>Sagwa</t>
+  </si>
+  <si>
+    <t>Edjian Prince</t>
+  </si>
+  <si>
+    <t>HarrGick</t>
+  </si>
+  <si>
+    <t>Quay Tolsite</t>
+  </si>
+  <si>
+    <t>Karjj</t>
+  </si>
+  <si>
+    <t>Lexi</t>
+  </si>
+  <si>
+    <t>Jagleo</t>
+  </si>
+  <si>
+    <t>Taraja Cuttsmay</t>
+  </si>
+  <si>
+    <t>Pashevir Duine</t>
+  </si>
+  <si>
+    <t>Gillen Finders</t>
+  </si>
+  <si>
+    <t>Jabba Desilijic Tiure</t>
+  </si>
+  <si>
+    <t>LeKelf</t>
+  </si>
+  <si>
+    <t>Cosdra</t>
+  </si>
+  <si>
+    <t>B8G-H0R</t>
+  </si>
+  <si>
+    <t>Chewbacca</t>
+  </si>
+  <si>
+    <t>Mattiso Trodu</t>
+  </si>
+  <si>
+    <t>Gorji Sandem</t>
+  </si>
+  <si>
+    <t>Aurodia Ventafoli</t>
+  </si>
+  <si>
+    <t>Dryden Vos</t>
+  </si>
+  <si>
+    <t>Bolandin</t>
+  </si>
+  <si>
+    <t>Boshti Anilee</t>
+  </si>
+  <si>
+    <t>L3-37</t>
+  </si>
+  <si>
+    <t>Gafferky Lenzwin</t>
+  </si>
+  <si>
+    <t>MK5-L1</t>
+  </si>
+  <si>
+    <t>Maul</t>
+  </si>
+  <si>
+    <t>Batcha Hunaris</t>
+  </si>
+  <si>
+    <t>Lando Calrissian's father</t>
+  </si>
+  <si>
+    <t>T1M8-LT2</t>
+  </si>
+  <si>
+    <t>Bink Otauna</t>
+  </si>
+  <si>
+    <t>Margo (Imroosian)</t>
+  </si>
+  <si>
+    <t>P6B-LT2</t>
+  </si>
+  <si>
+    <t>Regineer Teed</t>
+  </si>
+  <si>
+    <t>Qi'ra</t>
+  </si>
+  <si>
+    <t>Moloch</t>
+  </si>
+  <si>
+    <t>Bokret Humphreys</t>
+  </si>
+  <si>
+    <t>Drawd Munbrin</t>
+  </si>
+  <si>
+    <t>Ballia Noaddo</t>
+  </si>
+  <si>
+    <t>Vell Brank</t>
+  </si>
+  <si>
+    <t>Dobarn Tren</t>
+  </si>
+  <si>
+    <t>Auromae Iselo</t>
+  </si>
+  <si>
+    <t>Hado Gwin</t>
+  </si>
+  <si>
+    <t>Aurra Sing</t>
+  </si>
+  <si>
+    <t>Chussido</t>
+  </si>
+  <si>
+    <t>JBLX-24</t>
+  </si>
+  <si>
+    <t>Sharlu Greslin</t>
+  </si>
+  <si>
+    <t>Silvasu Fi</t>
+  </si>
+  <si>
+    <t>Yorsh Manted</t>
+  </si>
+  <si>
+    <t>Staz</t>
+  </si>
+  <si>
+    <t>R2-S8</t>
+  </si>
+  <si>
+    <t>Bossk</t>
+  </si>
+  <si>
+    <t>Falthina Sharest</t>
+  </si>
+  <si>
+    <t>Callixido Ryss</t>
+  </si>
+  <si>
+    <t>P4T-GM</t>
+  </si>
+  <si>
+    <t>Kara Safwan</t>
+  </si>
+  <si>
+    <t>Tayshin Maxa</t>
+  </si>
+  <si>
+    <t>Jannitha Xoczuko</t>
+  </si>
+  <si>
+    <t>Weazel</t>
+  </si>
+  <si>
+    <t>Pruno Jant</t>
+  </si>
+  <si>
+    <t>Tag Greenley</t>
+  </si>
+  <si>
+    <t>PA-LT4</t>
+  </si>
+  <si>
+    <t>Zuzanu Latt</t>
+  </si>
+  <si>
+    <t>Lost King of Duro</t>
+  </si>
+  <si>
+    <t>Blysto Noxton</t>
+  </si>
+  <si>
+    <t>Aemon Gremm</t>
+  </si>
+  <si>
+    <t>CC-4M</t>
+  </si>
+  <si>
+    <t>Tam Posla</t>
+  </si>
+  <si>
+    <t>Keela Hevis</t>
+  </si>
+  <si>
+    <t>Xodell</t>
+  </si>
+  <si>
+    <t>Naley Frifa</t>
+  </si>
+  <si>
+    <t>Lark and Jonk</t>
+  </si>
+  <si>
+    <t>Han Solo's father</t>
+  </si>
+  <si>
+    <t>Collum Woslo</t>
+  </si>
+  <si>
+    <t>Susaut Volupicite</t>
+  </si>
+  <si>
+    <t>Benthic</t>
+  </si>
+  <si>
+    <t>Krysguld Dartis</t>
+  </si>
+  <si>
+    <t>Darth Sidious</t>
+  </si>
+  <si>
+    <t>Diles Anevi</t>
+  </si>
+  <si>
+    <t>Moda Maxa</t>
+  </si>
+  <si>
+    <t>Crodit</t>
+  </si>
+  <si>
+    <t>R2-F1P</t>
+  </si>
+  <si>
+    <t>Glaucus</t>
+  </si>
+  <si>
+    <t>R5-232</t>
+  </si>
+  <si>
+    <t>J3-55</t>
+  </si>
+  <si>
+    <t>Iothene Jacontro</t>
+  </si>
+  <si>
+    <t>Luleo Primoc</t>
+  </si>
+  <si>
+    <t>Baxin Winstoll</t>
+  </si>
+  <si>
+    <t>Syke (White Worms)</t>
+  </si>
+  <si>
+    <t>Chakobi Sanwright</t>
+  </si>
+  <si>
+    <t>Bansee</t>
+  </si>
+  <si>
     <t>Dok-Ondar</t>
   </si>
   <si>
-    <t>Argus Panox</t>
-  </si>
-  <si>
-    <t>R5-PHT</t>
-  </si>
-  <si>
-    <t>Chates</t>
-  </si>
-  <si>
-    <t>Denwade Banevans</t>
-  </si>
-  <si>
-    <t>Needles</t>
-  </si>
-  <si>
-    <t>Waria Junus</t>
-  </si>
-  <si>
-    <t>HT-IN-4</t>
-  </si>
-  <si>
-    <t>Wesger Odry</t>
-  </si>
-  <si>
-    <t>Toht Ra</t>
-  </si>
-  <si>
-    <t>GOUD-4</t>
-  </si>
-  <si>
-    <t>Rio Durant</t>
-  </si>
-  <si>
-    <t>Fugas Fandita</t>
-  </si>
-  <si>
-    <t>Dava Cassamam</t>
-  </si>
-  <si>
-    <t>Crev Bombaasa</t>
-  </si>
-  <si>
-    <t>Ralakili</t>
-  </si>
-  <si>
-    <t>Tobias Beckett</t>
-  </si>
-  <si>
-    <t>Hallon</t>
-  </si>
-  <si>
-    <t>Therm Scissorpunch</t>
-  </si>
-  <si>
-    <t>Ottilie</t>
-  </si>
-  <si>
-    <t>Enfys Nest</t>
-  </si>
-  <si>
-    <t>Damici Stalado</t>
-  </si>
-  <si>
-    <t>1MSE-KUP24</t>
-  </si>
-  <si>
-    <t>Odeffro Msern</t>
-  </si>
-  <si>
-    <t>Han Solo</t>
-  </si>
-  <si>
-    <t>Tak</t>
-  </si>
-  <si>
-    <t>Senna (Gigoran)</t>
-  </si>
-  <si>
-    <t>Proxima</t>
-  </si>
-  <si>
-    <t>Loru Denholt</t>
-  </si>
-  <si>
-    <t>Sinuth</t>
-  </si>
-  <si>
-    <t>Gelan Yees</t>
-  </si>
-  <si>
-    <t>Sagwa</t>
-  </si>
-  <si>
-    <t>Edjian Prince</t>
-  </si>
-  <si>
-    <t>HarrGick</t>
-  </si>
-  <si>
-    <t>Quay Tolsite</t>
-  </si>
-  <si>
-    <t>Karjj</t>
-  </si>
-  <si>
-    <t>Lexi</t>
-  </si>
-  <si>
-    <t>Jagleo</t>
-  </si>
-  <si>
-    <t>Taraja Cuttsmay</t>
-  </si>
-  <si>
-    <t>Pashevir Duine</t>
-  </si>
-  <si>
-    <t>Gillen Finders</t>
-  </si>
-  <si>
-    <t>Jabba Desilijic Tiure</t>
-  </si>
-  <si>
-    <t>LeKelf</t>
-  </si>
-  <si>
-    <t>Cosdra</t>
-  </si>
-  <si>
-    <t>B8G-H0R</t>
-  </si>
-  <si>
-    <t>Chewbacca</t>
-  </si>
-  <si>
-    <t>Mattiso Trodu</t>
-  </si>
-  <si>
-    <t>Gorji Sandem</t>
-  </si>
-  <si>
-    <t>Weazel</t>
-  </si>
-  <si>
-    <t>Aurodia Ventafoli</t>
-  </si>
-  <si>
-    <t>Dryden Vos</t>
-  </si>
-  <si>
-    <t>Bolandin</t>
-  </si>
-  <si>
-    <t>Boshti Anilee</t>
-  </si>
-  <si>
-    <t>L3-37</t>
-  </si>
-  <si>
-    <t>Gafferky Lenzwin</t>
-  </si>
-  <si>
-    <t>MK5-L1</t>
-  </si>
-  <si>
-    <t>Maul</t>
-  </si>
-  <si>
-    <t>Batcha Hunaris</t>
-  </si>
-  <si>
-    <t>Lando Calrissian's father</t>
-  </si>
-  <si>
-    <t>T1M8-LT2</t>
-  </si>
-  <si>
-    <t>Bink Otauna</t>
-  </si>
-  <si>
-    <t>Margo (Imroosian)</t>
-  </si>
-  <si>
-    <t>P6B-LT2</t>
-  </si>
-  <si>
-    <t>Regineer Teed</t>
-  </si>
-  <si>
-    <t>Qi'ra</t>
-  </si>
-  <si>
-    <t>Moloch</t>
-  </si>
-  <si>
-    <t>Bokret Humphreys</t>
-  </si>
-  <si>
-    <t>Drawd Munbrin</t>
-  </si>
-  <si>
-    <t>Ballia Noaddo</t>
-  </si>
-  <si>
-    <t>Vell Brank</t>
-  </si>
-  <si>
-    <t>Dobarn Tren</t>
-  </si>
-  <si>
-    <t>Auromae Iselo</t>
-  </si>
-  <si>
-    <t>Hado Gwin</t>
-  </si>
-  <si>
-    <t>Aurra Sing</t>
-  </si>
-  <si>
-    <t>Chussido</t>
-  </si>
-  <si>
-    <t>JBLX-24</t>
-  </si>
-  <si>
-    <t>Sharlu Greslin</t>
-  </si>
-  <si>
-    <t>Silvasu Fi</t>
-  </si>
-  <si>
-    <t>Yorsh Manted</t>
-  </si>
-  <si>
-    <t>Staz</t>
-  </si>
-  <si>
-    <t>R2-S8</t>
-  </si>
-  <si>
-    <t>Bossk</t>
-  </si>
-  <si>
-    <t>Falthina Sharest</t>
-  </si>
-  <si>
-    <t>Callixido Ryss</t>
-  </si>
-  <si>
-    <t>P4T-GM</t>
-  </si>
-  <si>
-    <t>Kara Safwan</t>
-  </si>
-  <si>
-    <t>Tayshin Maxa</t>
-  </si>
-  <si>
-    <t>Jannitha Xoczuko</t>
+    <t>Ardwyl Hercho</t>
   </si>
   <si>
     <t>Danith Nodar</t>
-  </si>
-  <si>
-    <t>Pruno Jant</t>
-  </si>
-  <si>
-    <t>Tag Greenley</t>
-  </si>
-  <si>
-    <t>PA-LT4</t>
-  </si>
-  <si>
-    <t>Zuzanu Latt</t>
-  </si>
-  <si>
-    <t>Lost King of Duro</t>
-  </si>
-  <si>
-    <t>Blysto Noxton</t>
-  </si>
-  <si>
-    <t>Aemon Gremm</t>
-  </si>
-  <si>
-    <t>R5-232</t>
-  </si>
-  <si>
-    <t>Tam Posla</t>
-  </si>
-  <si>
-    <t>Keela Hevis</t>
-  </si>
-  <si>
-    <t>Xodell</t>
-  </si>
-  <si>
-    <t>Naley Frifa</t>
-  </si>
-  <si>
-    <t>Lark and Jonk</t>
-  </si>
-  <si>
-    <t>Han Solo's father</t>
-  </si>
-  <si>
-    <t>Collum Woslo</t>
-  </si>
-  <si>
-    <t>Susaut Volupicite</t>
-  </si>
-  <si>
-    <t>Benthic</t>
-  </si>
-  <si>
-    <t>Krysguld Dartis</t>
-  </si>
-  <si>
-    <t>Darth Sidious</t>
-  </si>
-  <si>
-    <t>Diles Anevi</t>
-  </si>
-  <si>
-    <t>Moda Maxa</t>
-  </si>
-  <si>
-    <t>Crodit</t>
-  </si>
-  <si>
-    <t>R2-F1P</t>
-  </si>
-  <si>
-    <t>Glaucus</t>
-  </si>
-  <si>
-    <t>CC-4M</t>
-  </si>
-  <si>
-    <t>J3-55</t>
-  </si>
-  <si>
-    <t>Iothene Jacontro</t>
-  </si>
-  <si>
-    <t>Luleo Primoc</t>
-  </si>
-  <si>
-    <t>Baxin Winstoll</t>
-  </si>
-  <si>
-    <t>Syke (White Worms)</t>
-  </si>
-  <si>
-    <t>Chakobi Sanwright</t>
-  </si>
-  <si>
-    <t>Bansee</t>
-  </si>
-  <si>
-    <t>Rebolt</t>
-  </si>
-  <si>
-    <t>Ardwyl Hercho</t>
   </si>
   <si>
     <t>Attichitcuk</t>
@@ -833,13 +839,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F150"/>
+  <dimension ref="A1:H150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -855,8 +861,14 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -872,11 +884,17 @@
       <c r="E2">
         <v>0.1694133688854272</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -892,11 +910,17 @@
       <c r="E3">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -912,11 +936,17 @@
       <c r="E4">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -932,11 +962,17 @@
       <c r="E5">
         <v>0.3090895260188857</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="F5">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -952,11 +988,17 @@
       <c r="E6">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -972,11 +1014,17 @@
       <c r="E7">
         <v>0.02911493439227036</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -992,11 +1040,17 @@
       <c r="E8">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1012,11 +1066,17 @@
       <c r="E9">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1032,11 +1092,17 @@
       <c r="E10">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1052,11 +1118,17 @@
       <c r="E11">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1072,11 +1144,17 @@
       <c r="E12">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1092,31 +1170,43 @@
       <c r="E13">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.0002030091315805601</v>
       </c>
       <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>0.05405405405405406</v>
+      </c>
+      <c r="E14">
+        <v>0.0004047570973535294</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14">
         <v>5</v>
       </c>
-      <c r="D14">
-        <v>0.03378378378378379</v>
-      </c>
-      <c r="E14">
-        <v>1.046426383685005e-10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1132,11 +1222,17 @@
       <c r="E15">
         <v>9.741278335394956e-09</v>
       </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1152,11 +1248,17 @@
       <c r="E16">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1172,11 +1274,17 @@
       <c r="E17">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1192,11 +1300,17 @@
       <c r="E18">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1212,11 +1326,17 @@
       <c r="E19">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1232,11 +1352,17 @@
       <c r="E20">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1252,11 +1378,17 @@
       <c r="E21">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1272,11 +1404,17 @@
       <c r="E22">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1292,11 +1430,17 @@
       <c r="E23">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1312,11 +1456,17 @@
       <c r="E24">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1332,11 +1482,17 @@
       <c r="E25">
         <v>0.1701999244757633</v>
       </c>
-      <c r="F25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1352,11 +1508,17 @@
       <c r="E26">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1372,11 +1534,17 @@
       <c r="E27">
         <v>9.741278335394956e-09</v>
       </c>
-      <c r="F27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1392,11 +1560,17 @@
       <c r="E28">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1412,11 +1586,17 @@
       <c r="E29">
         <v>0.02457439955975476</v>
       </c>
-      <c r="F29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1432,11 +1612,17 @@
       <c r="E30">
         <v>0.3496806686848532</v>
       </c>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="F30">
+        <v>29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1452,11 +1638,17 @@
       <c r="E31">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1472,11 +1664,17 @@
       <c r="E32">
         <v>9.836408006639048e-09</v>
       </c>
-      <c r="F32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1492,11 +1690,17 @@
       <c r="E33">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
+      <c r="H33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1510,13 +1714,19 @@
         <v>0.1824324324324325</v>
       </c>
       <c r="E34">
-        <v>0.2644509276289796</v>
-      </c>
-      <c r="F34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>0.2644509276289795</v>
+      </c>
+      <c r="F34">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1532,11 +1742,17 @@
       <c r="E35">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F35" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>40</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1552,11 +1768,17 @@
       <c r="E36">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F36" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1572,11 +1794,17 @@
       <c r="E37">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1592,11 +1820,17 @@
       <c r="E38">
         <v>0.3934297679761389</v>
       </c>
-      <c r="F38" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="F38">
+        <v>62</v>
+      </c>
+      <c r="G38" t="s">
+        <v>43</v>
+      </c>
+      <c r="H38">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1612,11 +1846,17 @@
       <c r="E39">
         <v>0.007946558856476637</v>
       </c>
-      <c r="F39" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>44</v>
+      </c>
+      <c r="H39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1632,11 +1872,17 @@
       <c r="E40">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F40" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1652,11 +1898,17 @@
       <c r="E41">
         <v>0.1079026617775398</v>
       </c>
-      <c r="F41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="F41">
+        <v>14</v>
+      </c>
+      <c r="G41" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1672,11 +1924,17 @@
       <c r="E42">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F42" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1692,11 +1950,17 @@
       <c r="E43">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1712,11 +1976,17 @@
       <c r="E44">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F44" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1732,11 +2002,17 @@
       <c r="E45">
         <v>0.007158224874014489</v>
       </c>
-      <c r="F45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>50</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1752,11 +2028,17 @@
       <c r="E46">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F46" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
+        <v>51</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1772,11 +2054,17 @@
       <c r="E47">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>52</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1792,11 +2080,17 @@
       <c r="E48">
         <v>0.06501294527183177</v>
       </c>
-      <c r="F48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="F48">
+        <v>6</v>
+      </c>
+      <c r="G48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1812,11 +2106,17 @@
       <c r="E49">
         <v>9.741278335394956e-09</v>
       </c>
-      <c r="F49" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1832,11 +2132,17 @@
       <c r="E50">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F50" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1852,11 +2158,17 @@
       <c r="E51">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F51" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
+        <v>56</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1872,11 +2184,17 @@
       <c r="E52">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F52" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>57</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1892,11 +2210,17 @@
       <c r="E53">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
+        <v>58</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1912,11 +2236,17 @@
       <c r="E54">
         <v>9.741278335394956e-09</v>
       </c>
-      <c r="F54" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" t="s">
+        <v>59</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1932,11 +2262,17 @@
       <c r="E55">
         <v>0.2346403082861319</v>
       </c>
-      <c r="F55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="F55">
+        <v>9</v>
+      </c>
+      <c r="G55" t="s">
+        <v>60</v>
+      </c>
+      <c r="H55">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1952,11 +2288,17 @@
       <c r="E56">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56" t="s">
+        <v>61</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1972,11 +2314,17 @@
       <c r="E57">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F57" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1992,16 +2340,22 @@
       <c r="E58">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F58" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58" t="s">
+        <v>63</v>
+      </c>
+      <c r="H58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59">
-        <v>0.0141973772075813</v>
+        <v>0.01419737720758129</v>
       </c>
       <c r="C59">
         <v>34</v>
@@ -2012,11 +2366,17 @@
       <c r="E59">
         <v>0.2959003854113182</v>
       </c>
-      <c r="F59" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="F59">
+        <v>23</v>
+      </c>
+      <c r="G59" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2032,11 +2392,17 @@
       <c r="E60">
         <v>9.741278335394956e-09</v>
       </c>
-      <c r="F60" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>65</v>
+      </c>
+      <c r="H60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2052,71 +2418,95 @@
       <c r="E61">
         <v>9.741278335394956e-09</v>
       </c>
-      <c r="F61" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
+        <v>66</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62">
-        <v>0.01056026872353403</v>
+        <v>0.001746644603787461</v>
       </c>
       <c r="C62">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D62">
-        <v>0.08783783783783784</v>
+        <v>0.04054054054054054</v>
       </c>
       <c r="E62">
-        <v>0.02911493439227036</v>
-      </c>
-      <c r="F62" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6">
+        <v>1.16885827057615e-07</v>
+      </c>
+      <c r="F62">
+        <v>4</v>
+      </c>
+      <c r="G62" t="s">
+        <v>67</v>
+      </c>
+      <c r="H62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63">
-        <v>0.001746644603787461</v>
+        <v>0.03936460314011331</v>
       </c>
       <c r="C63">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="D63">
-        <v>0.04054054054054054</v>
+        <v>0.3108108108108109</v>
       </c>
       <c r="E63">
-        <v>1.16885827057615e-07</v>
-      </c>
-      <c r="F63" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
+        <v>0.3207714249519975</v>
+      </c>
+      <c r="F63">
+        <v>32</v>
+      </c>
+      <c r="G63" t="s">
+        <v>68</v>
+      </c>
+      <c r="H63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64">
-        <v>0.03936460314011332</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="D64">
-        <v>0.3108108108108109</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E64">
-        <v>0.3207714249519975</v>
-      </c>
-      <c r="F64" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64" t="s">
+        <v>69</v>
+      </c>
+      <c r="H64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2124,59 +2514,77 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D65">
-        <v>0.01351351351351351</v>
+        <v>0.03378378378378379</v>
       </c>
       <c r="E65">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>9.741278335394956e-09</v>
+      </c>
+      <c r="F65">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
+        <v>70</v>
+      </c>
+      <c r="H65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>0.02990608551833041</v>
       </c>
       <c r="C66">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D66">
-        <v>0.03378378378378379</v>
+        <v>0.2094594594594595</v>
       </c>
       <c r="E66">
-        <v>9.741278335394956e-09</v>
-      </c>
-      <c r="F66" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>0.2232074318250236</v>
+      </c>
+      <c r="F66">
+        <v>25</v>
+      </c>
+      <c r="G66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67">
-        <v>0.02990608551833041</v>
+        <v>0</v>
       </c>
       <c r="C67">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="D67">
-        <v>0.2094594594594595</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E67">
-        <v>0.2232074318250236</v>
-      </c>
-      <c r="F67" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67" t="s">
+        <v>72</v>
+      </c>
+      <c r="H67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2184,59 +2592,77 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D68">
-        <v>0.01351351351351351</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E68">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F68" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>73</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>0.00193363088771252</v>
       </c>
       <c r="C69">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="D69">
-        <v>0.006756756756756757</v>
+        <v>0.1081081081081081</v>
       </c>
       <c r="E69">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F69" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
+        <v>0.2375616055295733</v>
+      </c>
+      <c r="F69">
+        <v>8</v>
+      </c>
+      <c r="G69" t="s">
+        <v>74</v>
+      </c>
+      <c r="H69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70">
-        <v>0.00193363088771252</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D70">
-        <v>0.1081081081081081</v>
+        <v>0.04054054054054054</v>
       </c>
       <c r="E70">
-        <v>0.2375616055295733</v>
-      </c>
-      <c r="F70" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70" t="s">
+        <v>75</v>
+      </c>
+      <c r="H70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2244,19 +2670,25 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D71">
-        <v>0.04054054054054054</v>
+        <v>0.02027027027027027</v>
       </c>
       <c r="E71">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F71" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71" t="s">
+        <v>76</v>
+      </c>
+      <c r="H71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2264,19 +2696,25 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D72">
-        <v>0.02027027027027027</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E72">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F72" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72" t="s">
+        <v>77</v>
+      </c>
+      <c r="H72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2292,51 +2730,69 @@
       <c r="E73">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F73" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6">
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73" t="s">
+        <v>78</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>0.01045688545688546</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D74">
-        <v>0.006756756756756757</v>
+        <v>0.06081081081081081</v>
       </c>
       <c r="E74">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F74" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
+        <v>0.02917613269867489</v>
+      </c>
+      <c r="F74">
+        <v>2</v>
+      </c>
+      <c r="G74" t="s">
+        <v>79</v>
+      </c>
+      <c r="H74">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75">
-        <v>0.01045688545688546</v>
+        <v>0</v>
       </c>
       <c r="C75">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>0.06081081081081081</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E75">
-        <v>0.02917613269867489</v>
-      </c>
-      <c r="F75" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>80</v>
+      </c>
+      <c r="H75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2344,79 +2800,103 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>0.006756756756756757</v>
+        <v>0</v>
       </c>
       <c r="E76">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F76" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76" t="s">
+        <v>81</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.04544290513678272</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>0.2635135135135135</v>
       </c>
       <c r="E77">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F77" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
+        <v>0.2617855293629051</v>
+      </c>
+      <c r="F77">
+        <v>26</v>
+      </c>
+      <c r="G77" t="s">
+        <v>82</v>
+      </c>
+      <c r="H77">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0.04544290513678271</v>
+        <v>0.009943617086474231</v>
       </c>
       <c r="C78">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D78">
-        <v>0.2635135135135135</v>
+        <v>0.05405405405405406</v>
       </c>
       <c r="E78">
-        <v>0.2617855293629052</v>
-      </c>
-      <c r="F78" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
+        <v>0.003263508246721235</v>
+      </c>
+      <c r="F78">
+        <v>3</v>
+      </c>
+      <c r="G78" t="s">
+        <v>83</v>
+      </c>
+      <c r="H78">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0.009943617086474231</v>
+        <v>0</v>
       </c>
       <c r="C79">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D79">
-        <v>0.05405405405405406</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E79">
-        <v>0.003263508246721234</v>
-      </c>
-      <c r="F79" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
+        <v>9.741278335394956e-09</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79" t="s">
+        <v>84</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2430,13 +2910,19 @@
         <v>0.01351351351351351</v>
       </c>
       <c r="E80">
-        <v>9.741278335394956e-09</v>
-      </c>
-      <c r="F80" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
+        <v>0.04331523403660618</v>
+      </c>
+      <c r="F80">
+        <v>1</v>
+      </c>
+      <c r="G80" t="s">
+        <v>85</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2444,19 +2930,25 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>0.01351351351351351</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>0.04331523403660618</v>
-      </c>
-      <c r="F81" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81" t="s">
+        <v>86</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2472,11 +2964,17 @@
       <c r="E82">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F82" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82" t="s">
+        <v>87</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2484,19 +2982,25 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E83">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F83" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83" t="s">
+        <v>88</v>
+      </c>
+      <c r="H83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2504,19 +3008,25 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84">
-        <v>0.01351351351351351</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E84">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F84" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s">
+        <v>89</v>
+      </c>
+      <c r="H84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2524,59 +3034,77 @@
         <v>0</v>
       </c>
       <c r="C85">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D85">
-        <v>0.006756756756756757</v>
+        <v>0.03378378378378379</v>
       </c>
       <c r="E85">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F85" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
+        <v>9.741278335394956e-09</v>
+      </c>
+      <c r="F85">
+        <v>1</v>
+      </c>
+      <c r="G85" t="s">
+        <v>90</v>
+      </c>
+      <c r="H85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>0.005140234987173762</v>
       </c>
       <c r="C86">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D86">
-        <v>0.03378378378378379</v>
+        <v>0.06756756756756757</v>
       </c>
       <c r="E86">
-        <v>9.741278335394956e-09</v>
-      </c>
-      <c r="F86" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>0.1011919684487238</v>
+      </c>
+      <c r="F86">
+        <v>4</v>
+      </c>
+      <c r="G86" t="s">
+        <v>91</v>
+      </c>
+      <c r="H86">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87">
-        <v>0.005140234987173762</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D87">
-        <v>0.06756756756756757</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E87">
-        <v>0.1011919684487238</v>
-      </c>
-      <c r="F87" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>92</v>
+      </c>
+      <c r="H87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2592,11 +3120,17 @@
       <c r="E88">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F88" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88" t="s">
+        <v>93</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2604,19 +3138,25 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>0.006756756756756757</v>
+        <v>0</v>
       </c>
       <c r="E89">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F89" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89" t="s">
+        <v>94</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2632,11 +3172,17 @@
       <c r="E90">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F90" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>95</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2644,19 +3190,25 @@
         <v>0</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>0.02702702702702703</v>
       </c>
       <c r="E91">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F91" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
+        <v>96</v>
+      </c>
+      <c r="H91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2664,19 +3216,25 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D92">
-        <v>0.02702702702702703</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E92">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F92" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92" t="s">
+        <v>97</v>
+      </c>
+      <c r="H92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2684,64 +3242,82 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>0.01351351351351351</v>
+        <v>0</v>
       </c>
       <c r="E93">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F93" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93" t="s">
+        <v>98</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>0.0001294662008947723</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>0.05405405405405406</v>
       </c>
       <c r="E94">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F94" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
+        <v>0.01113980406165391</v>
+      </c>
+      <c r="F94">
+        <v>1</v>
+      </c>
+      <c r="G94" t="s">
+        <v>99</v>
+      </c>
+      <c r="H94">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95">
-        <v>0.0001294662008947723</v>
+        <v>0.01475455046883618</v>
       </c>
       <c r="C95">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D95">
-        <v>0.05405405405405406</v>
+        <v>0.03378378378378379</v>
       </c>
       <c r="E95">
-        <v>0.01113980406165391</v>
-      </c>
-      <c r="F95" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
+        <v>0.02882223975274039</v>
+      </c>
+      <c r="F95">
+        <v>2</v>
+      </c>
+      <c r="G95" t="s">
+        <v>100</v>
+      </c>
+      <c r="H95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96">
-        <v>0.01475455046883618</v>
+        <v>0.0001994341280055566</v>
       </c>
       <c r="C96">
         <v>5</v>
@@ -2750,33 +3326,45 @@
         <v>0.03378378378378379</v>
       </c>
       <c r="E96">
-        <v>0.02882223975274039</v>
-      </c>
-      <c r="F96" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
+        <v>0.003970632235850674</v>
+      </c>
+      <c r="F96">
+        <v>3</v>
+      </c>
+      <c r="G96" t="s">
+        <v>101</v>
+      </c>
+      <c r="H96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97">
-        <v>0.0001994341280055566</v>
+        <v>0</v>
       </c>
       <c r="C97">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D97">
-        <v>0.03378378378378379</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E97">
-        <v>0.003970632235850674</v>
-      </c>
-      <c r="F97" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" t="s">
+        <v>102</v>
+      </c>
+      <c r="H97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2784,79 +3372,103 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D98">
-        <v>0.006756756756756757</v>
+        <v>0.02027027027027027</v>
       </c>
       <c r="E98">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F98" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6">
+        <v>0.003212644114328134</v>
+      </c>
+      <c r="F98">
+        <v>1</v>
+      </c>
+      <c r="G98" t="s">
+        <v>103</v>
+      </c>
+      <c r="H98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>0.0005075228289514004</v>
       </c>
       <c r="C99">
+        <v>6</v>
+      </c>
+      <c r="D99">
+        <v>0.04054054054054054</v>
+      </c>
+      <c r="E99">
+        <v>0.002974174785813463</v>
+      </c>
+      <c r="F99">
         <v>3</v>
       </c>
-      <c r="D99">
-        <v>0.02027027027027027</v>
-      </c>
-      <c r="E99">
-        <v>0.003212644114328134</v>
-      </c>
-      <c r="F99" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6">
+      <c r="G99" t="s">
+        <v>104</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100">
-        <v>0.0005075228289514004</v>
+        <v>0</v>
       </c>
       <c r="C100">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>0.04054054054054054</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>0.002974174785813463</v>
-      </c>
-      <c r="F100" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100" t="s">
+        <v>105</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>0.01056026872353403</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>0.08783783783783784</v>
       </c>
       <c r="E101">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F101" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6">
+        <v>0.02911493439227036</v>
+      </c>
+      <c r="F101">
+        <v>1</v>
+      </c>
+      <c r="G101" t="s">
+        <v>106</v>
+      </c>
+      <c r="H101">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2872,11 +3484,17 @@
       <c r="E102">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F102" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6">
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102" t="s">
+        <v>107</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2884,19 +3502,25 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E103">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F103" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103" t="s">
+        <v>108</v>
+      </c>
+      <c r="H103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2912,51 +3536,69 @@
       <c r="E104">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F104" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6">
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104" t="s">
+        <v>109</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>0.001746644603787461</v>
       </c>
       <c r="C105">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D105">
-        <v>0.006756756756756757</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E105">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F105" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6">
+        <v>1.046426383685005e-10</v>
+      </c>
+      <c r="F105">
+        <v>1</v>
+      </c>
+      <c r="G105" t="s">
+        <v>110</v>
+      </c>
+      <c r="H105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106">
-        <v>0.001746644603787461</v>
+        <v>0</v>
       </c>
       <c r="C106">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D106">
-        <v>0.01351351351351351</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E106">
-        <v>1.046426383685005e-10</v>
-      </c>
-      <c r="F106" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106" t="s">
+        <v>111</v>
+      </c>
+      <c r="H106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2972,11 +3614,17 @@
       <c r="E107">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F107" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107" t="s">
+        <v>112</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2992,11 +3640,17 @@
       <c r="E108">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F108" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108" t="s">
+        <v>113</v>
+      </c>
+      <c r="H108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3012,11 +3666,17 @@
       <c r="E109">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F109" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109" t="s">
+        <v>114</v>
+      </c>
+      <c r="H109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3024,19 +3684,25 @@
         <v>0</v>
       </c>
       <c r="C110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D110">
-        <v>0.02027027027027027</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E110">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F110" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>115</v>
+      </c>
+      <c r="H110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3044,19 +3710,25 @@
         <v>0</v>
       </c>
       <c r="C111">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>0.01351351351351351</v>
+        <v>0</v>
       </c>
       <c r="E111">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F111" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6">
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111" t="s">
+        <v>116</v>
+      </c>
+      <c r="H111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3072,11 +3744,17 @@
       <c r="E112">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F112" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112" t="s">
+        <v>117</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3092,11 +3770,17 @@
       <c r="E113">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F113" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113" t="s">
+        <v>118</v>
+      </c>
+      <c r="H113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3104,19 +3788,25 @@
         <v>0</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E114">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F114" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+        <v>9.741278335394956e-09</v>
+      </c>
+      <c r="F114">
+        <v>1</v>
+      </c>
+      <c r="G114" t="s">
+        <v>119</v>
+      </c>
+      <c r="H114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3124,19 +3814,25 @@
         <v>0</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D115">
-        <v>0.01351351351351351</v>
+        <v>0.02702702702702703</v>
       </c>
       <c r="E115">
-        <v>9.741278335394956e-09</v>
-      </c>
-      <c r="F115" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6">
+        <v>0.04331523413173585</v>
+      </c>
+      <c r="F115">
+        <v>2</v>
+      </c>
+      <c r="G115" t="s">
+        <v>120</v>
+      </c>
+      <c r="H115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3144,19 +3840,25 @@
         <v>0</v>
       </c>
       <c r="C116">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>0.02702702702702703</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>0.04331523413173585</v>
-      </c>
-      <c r="F116" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116" t="s">
+        <v>121</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3164,19 +3866,25 @@
         <v>0</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>0.02027027027027027</v>
       </c>
       <c r="E117">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F117" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6">
+      <c r="F117">
+        <v>0</v>
+      </c>
+      <c r="G117" t="s">
+        <v>122</v>
+      </c>
+      <c r="H117">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3190,13 +3898,19 @@
         <v>0.02027027027027027</v>
       </c>
       <c r="E118">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F118" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6">
+        <v>0.04331523403660618</v>
+      </c>
+      <c r="F118">
+        <v>1</v>
+      </c>
+      <c r="G118" t="s">
+        <v>123</v>
+      </c>
+      <c r="H118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3204,99 +3918,129 @@
         <v>0</v>
       </c>
       <c r="C119">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D119">
-        <v>0.02027027027027027</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E119">
-        <v>0.04331523403660618</v>
-      </c>
-      <c r="F119" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119" t="s">
+        <v>124</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>0.0001594375318865115</v>
       </c>
       <c r="C120">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D120">
-        <v>0.006756756756756757</v>
+        <v>0.08108108108108109</v>
       </c>
       <c r="E120">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F120" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
+        <v>0.2004245769436167</v>
+      </c>
+      <c r="F120">
+        <v>7</v>
+      </c>
+      <c r="G120" t="s">
+        <v>125</v>
+      </c>
+      <c r="H120">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121">
-        <v>0.0001594375318865115</v>
+        <v>0</v>
       </c>
       <c r="C121">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D121">
-        <v>0.08108108108108109</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E121">
-        <v>0.2004245769436167</v>
-      </c>
-      <c r="F121" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
+        <v>0.003212644114328134</v>
+      </c>
+      <c r="F121">
+        <v>1</v>
+      </c>
+      <c r="G121" t="s">
+        <v>126</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>0.001820825927968785</v>
       </c>
       <c r="C122">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D122">
-        <v>0.01351351351351351</v>
+        <v>0.04054054054054054</v>
       </c>
       <c r="E122">
-        <v>0.003212644114328134</v>
-      </c>
-      <c r="F122" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
+        <v>0.003970632235850674</v>
+      </c>
+      <c r="F122">
+        <v>3</v>
+      </c>
+      <c r="G122" t="s">
+        <v>127</v>
+      </c>
+      <c r="H122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123">
-        <v>0.001820825927968785</v>
+        <v>0</v>
       </c>
       <c r="C123">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>0.04054054054054054</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>0.003970632235850674</v>
-      </c>
-      <c r="F123" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F123">
+        <v>0</v>
+      </c>
+      <c r="G123" t="s">
+        <v>128</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3312,51 +4056,69 @@
       <c r="E124">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F124" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124" t="s">
+        <v>129</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>0.001930501930501931</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>0.05405405405405406</v>
       </c>
       <c r="E125">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F125" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
+        <v>9.741278335394956e-09</v>
+      </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
+      <c r="G125" t="s">
+        <v>130</v>
+      </c>
+      <c r="H125">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126">
-        <v>0.001930501930501931</v>
+        <v>0</v>
       </c>
       <c r="C126">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D126">
-        <v>0.05405405405405406</v>
+        <v>0.02027027027027027</v>
       </c>
       <c r="E126">
-        <v>9.741278335394956e-09</v>
-      </c>
-      <c r="F126" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="G126" t="s">
+        <v>131</v>
+      </c>
+      <c r="H126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3372,11 +4134,17 @@
       <c r="E127">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F127" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
+      <c r="F127">
+        <v>0</v>
+      </c>
+      <c r="G127" t="s">
+        <v>132</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3384,19 +4152,25 @@
         <v>0</v>
       </c>
       <c r="C128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>0.006756756756756757</v>
+        <v>0</v>
       </c>
       <c r="E128">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F128" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128" t="s">
+        <v>133</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3404,19 +4178,25 @@
         <v>0</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>0.03378378378378379</v>
       </c>
       <c r="E129">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F129" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
+        <v>1.16885827057615e-07</v>
+      </c>
+      <c r="F129">
+        <v>4</v>
+      </c>
+      <c r="G129" t="s">
+        <v>134</v>
+      </c>
+      <c r="H129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3424,19 +4204,25 @@
         <v>0</v>
       </c>
       <c r="C130">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D130">
-        <v>0.03378378378378379</v>
+        <v>0.006756756756756757</v>
       </c>
       <c r="E130">
-        <v>1.16885827057615e-07</v>
-      </c>
-      <c r="F130" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130" t="s">
+        <v>135</v>
+      </c>
+      <c r="H130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3444,19 +4230,25 @@
         <v>0</v>
       </c>
       <c r="C131">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D131">
-        <v>0.006756756756756757</v>
+        <v>0.0472972972972973</v>
       </c>
       <c r="E131">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F131" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
+        <v>0.0004047570878405622</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+      <c r="G131" t="s">
+        <v>136</v>
+      </c>
+      <c r="H131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3464,19 +4256,25 @@
         <v>0</v>
       </c>
       <c r="C132">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D132">
-        <v>0.0472972972972973</v>
+        <v>0.01351351351351351</v>
       </c>
       <c r="E132">
-        <v>0.0004047570878405622</v>
-      </c>
-      <c r="F132" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
+        <v>1.947304370366551e-08</v>
+      </c>
+      <c r="F132">
+        <v>2</v>
+      </c>
+      <c r="G132" t="s">
+        <v>137</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3490,13 +4288,19 @@
         <v>0.01351351351351351</v>
       </c>
       <c r="E133">
-        <v>1.947304370366551e-08</v>
-      </c>
-      <c r="F133" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F133">
+        <v>0</v>
+      </c>
+      <c r="G133" t="s">
+        <v>138</v>
+      </c>
+      <c r="H133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3504,39 +4308,51 @@
         <v>0</v>
       </c>
       <c r="C134">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D134">
-        <v>0.01351351351351351</v>
+        <v>0.03378378378378379</v>
       </c>
       <c r="E134">
-        <v>9.512967124409137e-12</v>
-      </c>
-      <c r="F134" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6">
+        <v>1.046426383685005e-10</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="G134" t="s">
+        <v>139</v>
+      </c>
+      <c r="H134">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135" s="1">
         <v>133</v>
       </c>
       <c r="B135">
-        <v>0.0002030091315805601</v>
+        <v>0</v>
       </c>
       <c r="C135">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>0.05405405405405406</v>
+        <v>0</v>
       </c>
       <c r="E135">
-        <v>0.0004047570973535294</v>
-      </c>
-      <c r="F135" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6">
+        <v>9.512967124409137e-12</v>
+      </c>
+      <c r="F135">
+        <v>0</v>
+      </c>
+      <c r="G135" t="s">
+        <v>140</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3552,11 +4368,17 @@
       <c r="E136">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F136" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6">
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136" t="s">
+        <v>141</v>
+      </c>
+      <c r="H136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3572,11 +4394,17 @@
       <c r="E137">
         <v>0.03257597597666178</v>
       </c>
-      <c r="F137" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6">
+      <c r="F137">
+        <v>1</v>
+      </c>
+      <c r="G137" t="s">
+        <v>142</v>
+      </c>
+      <c r="H137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3592,11 +4420,17 @@
       <c r="E138">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F138" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6">
+      <c r="F138">
+        <v>0</v>
+      </c>
+      <c r="G138" t="s">
+        <v>143</v>
+      </c>
+      <c r="H138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3612,11 +4446,17 @@
       <c r="E139">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F139" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139" t="s">
+        <v>144</v>
+      </c>
+      <c r="H139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3632,11 +4472,17 @@
       <c r="E140">
         <v>0.04331523403660618</v>
       </c>
-      <c r="F140" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
+      <c r="F140">
+        <v>1</v>
+      </c>
+      <c r="G140" t="s">
+        <v>145</v>
+      </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3652,11 +4498,17 @@
       <c r="E141">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F141" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141" t="s">
+        <v>146</v>
+      </c>
+      <c r="H141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3672,11 +4524,17 @@
       <c r="E142">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F142" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142" t="s">
+        <v>147</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3692,11 +4550,17 @@
       <c r="E143">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F143" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143" t="s">
+        <v>148</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3712,11 +4576,17 @@
       <c r="E144">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F144" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144" t="s">
+        <v>149</v>
+      </c>
+      <c r="H144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3732,11 +4602,17 @@
       <c r="E145">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F145" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
+      <c r="F145">
+        <v>0</v>
+      </c>
+      <c r="G145" t="s">
+        <v>150</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3752,11 +4628,17 @@
       <c r="E146">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F146" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
+      <c r="F146">
+        <v>0</v>
+      </c>
+      <c r="G146" t="s">
+        <v>151</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3772,11 +4654,17 @@
       <c r="E147">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F147" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
+      <c r="F147">
+        <v>0</v>
+      </c>
+      <c r="G147" t="s">
+        <v>152</v>
+      </c>
+      <c r="H147">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3792,11 +4680,17 @@
       <c r="E148">
         <v>0.01906631223755011</v>
       </c>
-      <c r="F148" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
+      <c r="F148">
+        <v>3</v>
+      </c>
+      <c r="G148" t="s">
+        <v>153</v>
+      </c>
+      <c r="H148">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3812,11 +4706,17 @@
       <c r="E149">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F149" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149" t="s">
+        <v>154</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3832,8 +4732,14 @@
       <c r="E150">
         <v>9.512967124409137e-12</v>
       </c>
-      <c r="F150" t="s">
-        <v>153</v>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150" t="s">
+        <v>155</v>
+      </c>
+      <c r="H150">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>